<commit_message>
playing around in excel
</commit_message>
<xml_diff>
--- a/data/raw/ADFG_strayrates.xlsx
+++ b/data/raw/ADFG_strayrates.xlsx
@@ -5,26 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\OneDrive\Documents\dissertation\SITK\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\OneDrive\Documents\dissertation\SITK\Github\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B29426-2DD4-4BDB-8301-6A706841E255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0087409-211D-40B4-A224-2D709A2CF88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{28766EB7-7A80-4306-B235-966A57E0829F}"/>
+    <workbookView xWindow="-52920" yWindow="-375" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{28766EB7-7A80-4306-B235-966A57E0829F}"/>
   </bookViews>
   <sheets>
     <sheet name="ADFG_strayrates" sheetId="1" r:id="rId1"/>
     <sheet name="cleaned" sheetId="2" r:id="rId2"/>
     <sheet name="statweek v. stray%" sheetId="3" r:id="rId3"/>
-    <sheet name="annual" sheetId="4" r:id="rId4"/>
-    <sheet name="timing" sheetId="6" r:id="rId5"/>
-    <sheet name="indian river returns" sheetId="5" r:id="rId6"/>
+    <sheet name="cost rec v. rack return" sheetId="7" r:id="rId4"/>
+    <sheet name="annual" sheetId="4" r:id="rId5"/>
+    <sheet name="timing" sheetId="6" r:id="rId6"/>
+    <sheet name="indian river returns" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">annual!$A$1:$P$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">annual!$A$1:$P$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'statweek v. stray%'!$A$1:$P$42</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">timing!$H$5</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">timing!$C$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1779" uniqueCount="105">
   <si>
     <t>Year</t>
   </si>
@@ -2439,6 +2438,465 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'cost rec v. rack return'!$I$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COST RECOVERY</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'cost rec v. rack return'!$J$20:$J$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'cost rec v. rack return'!$K$20:$K$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.65693430656934304</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77272727272727271</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88659793814432986</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95121951219512191</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3E93-4D40-9C7C-A7B7AA4AE421}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'cost rec v. rack return'!$I$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RACK RETURN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'cost rec v. rack return'!$J$26:$J$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'cost rec v. rack return'!$K$26:$K$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46376811594202899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57608695652173914</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23404255319148937</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18085106382978725</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.5106382978723402E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3E93-4D40-9C7C-A7B7AA4AE421}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1874176496"/>
+        <c:axId val="1874177456"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1874176496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="39"/>
+          <c:min val="29"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1874177456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1874177456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1874176496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2520,6 +2978,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4107,6 +4605,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4212,6 +5226,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>14286</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A928F4B-A5CF-5545-2269-6B6055DDA5F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11083,8 +12138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714CB146-BCCF-4F9B-B94D-0EAC1236C77C}">
   <dimension ref="A1:AG90"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection sqref="A1:P42"/>
+    <sheetView topLeftCell="A34" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:W90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15869,6 +16924,1655 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B33C61-2287-47AB-9433-641E2C9C08A2}">
+  <dimension ref="A1:W35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W33" sqref="W33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" t="s">
+        <v>84</v>
+      </c>
+      <c r="V1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" t="str">
+        <f t="shared" ref="W1:W17" si="0">U1</f>
+        <v>Mark%</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2024</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2">
+        <v>11341</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45514</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2">
+        <v>143</v>
+      </c>
+      <c r="L2">
+        <v>137</v>
+      </c>
+      <c r="M2">
+        <v>47</v>
+      </c>
+      <c r="N2">
+        <v>90</v>
+      </c>
+      <c r="O2">
+        <v>66</v>
+      </c>
+      <c r="P2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R2">
+        <v>47</v>
+      </c>
+      <c r="S2">
+        <v>90</v>
+      </c>
+      <c r="T2">
+        <f t="shared" ref="T2:T17" si="1">R2+S2</f>
+        <v>137</v>
+      </c>
+      <c r="U2">
+        <f t="shared" ref="U2:U17" si="2">S2/T2</f>
+        <v>0.65693430656934304</v>
+      </c>
+      <c r="V2">
+        <v>32</v>
+      </c>
+      <c r="W2">
+        <f t="shared" si="0"/>
+        <v>0.65693430656934304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2024</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <v>11341</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="1">
+        <v>45519</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3">
+        <v>142</v>
+      </c>
+      <c r="L3">
+        <v>135</v>
+      </c>
+      <c r="M3">
+        <v>54</v>
+      </c>
+      <c r="N3">
+        <v>81</v>
+      </c>
+      <c r="O3">
+        <v>60</v>
+      </c>
+      <c r="P3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3">
+        <v>54</v>
+      </c>
+      <c r="S3">
+        <v>81</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="V3">
+        <v>33</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <v>11341</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44442</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4">
+        <v>32</v>
+      </c>
+      <c r="L4">
+        <v>31</v>
+      </c>
+      <c r="M4">
+        <v>31</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>80</v>
+      </c>
+      <c r="R4">
+        <v>31</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>36</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2021</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>11341</v>
+      </c>
+      <c r="H5" s="1">
+        <v>44439</v>
+      </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5">
+        <v>35</v>
+      </c>
+      <c r="L5">
+        <v>32</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>29</v>
+      </c>
+      <c r="O5">
+        <v>91</v>
+      </c>
+      <c r="P5" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>29</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="2"/>
+        <v>0.90625</v>
+      </c>
+      <c r="V5">
+        <v>36</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="0"/>
+        <v>0.90625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2020</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>11341</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="1">
+        <v>44054</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6">
+        <v>96</v>
+      </c>
+      <c r="L6">
+        <v>66</v>
+      </c>
+      <c r="M6">
+        <v>15</v>
+      </c>
+      <c r="N6">
+        <v>51</v>
+      </c>
+      <c r="O6">
+        <v>77</v>
+      </c>
+      <c r="P6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R6">
+        <v>15</v>
+      </c>
+      <c r="S6">
+        <v>51</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="2"/>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="V6">
+        <v>33</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="0"/>
+        <v>0.77272727272727271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2019</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <v>11341</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1">
+        <v>43699</v>
+      </c>
+      <c r="I7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7">
+        <v>99</v>
+      </c>
+      <c r="L7">
+        <v>97</v>
+      </c>
+      <c r="M7">
+        <v>11</v>
+      </c>
+      <c r="N7">
+        <v>86</v>
+      </c>
+      <c r="O7">
+        <v>89</v>
+      </c>
+      <c r="P7" t="s">
+        <v>80</v>
+      </c>
+      <c r="R7">
+        <v>11</v>
+      </c>
+      <c r="S7">
+        <v>86</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="2"/>
+        <v>0.88659793814432986</v>
+      </c>
+      <c r="V7">
+        <v>34</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="0"/>
+        <v>0.88659793814432986</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2017</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>11341</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="1">
+        <v>42941</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8">
+        <v>86</v>
+      </c>
+      <c r="L8">
+        <v>82</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <v>78</v>
+      </c>
+      <c r="O8">
+        <v>95</v>
+      </c>
+      <c r="P8" t="s">
+        <v>80</v>
+      </c>
+      <c r="R8">
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <v>78</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="2"/>
+        <v>0.95121951219512191</v>
+      </c>
+      <c r="V8">
+        <v>30</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="0"/>
+        <v>0.95121951219512191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9">
+        <v>37</v>
+      </c>
+      <c r="E9">
+        <v>11341</v>
+      </c>
+      <c r="H9" s="1">
+        <v>42993</v>
+      </c>
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9">
+        <v>17</v>
+      </c>
+      <c r="L9">
+        <v>14</v>
+      </c>
+      <c r="M9">
+        <v>6</v>
+      </c>
+      <c r="N9">
+        <v>8</v>
+      </c>
+      <c r="O9">
+        <v>57</v>
+      </c>
+      <c r="P9" t="s">
+        <v>80</v>
+      </c>
+      <c r="R9">
+        <v>6</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="2"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="V9">
+        <v>37</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="0"/>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2017</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10">
+        <v>38</v>
+      </c>
+      <c r="E10">
+        <v>11341</v>
+      </c>
+      <c r="H10" s="1">
+        <v>42997</v>
+      </c>
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10">
+        <v>82</v>
+      </c>
+      <c r="L10">
+        <v>69</v>
+      </c>
+      <c r="M10">
+        <v>37</v>
+      </c>
+      <c r="N10">
+        <v>32</v>
+      </c>
+      <c r="O10">
+        <v>46</v>
+      </c>
+      <c r="P10" t="s">
+        <v>80</v>
+      </c>
+      <c r="R10">
+        <v>37</v>
+      </c>
+      <c r="S10">
+        <v>32</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="2"/>
+        <v>0.46376811594202899</v>
+      </c>
+      <c r="V10">
+        <v>38</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="0"/>
+        <v>0.46376811594202899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2016</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>34</v>
+      </c>
+      <c r="E11">
+        <v>11341</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="1">
+        <v>42596</v>
+      </c>
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11">
+        <v>50</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>46</v>
+      </c>
+      <c r="O11">
+        <v>92</v>
+      </c>
+      <c r="P11" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>46</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="2"/>
+        <v>0.92</v>
+      </c>
+      <c r="V11">
+        <v>34</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="0"/>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2016</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12">
+        <v>36</v>
+      </c>
+      <c r="E12">
+        <v>11341</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="1">
+        <v>42613</v>
+      </c>
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12">
+        <v>50</v>
+      </c>
+      <c r="L12">
+        <v>50</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>46</v>
+      </c>
+      <c r="O12">
+        <v>92</v>
+      </c>
+      <c r="P12" t="s">
+        <v>80</v>
+      </c>
+      <c r="R12">
+        <v>4</v>
+      </c>
+      <c r="S12">
+        <v>46</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="2"/>
+        <v>0.92</v>
+      </c>
+      <c r="V12">
+        <v>36</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="0"/>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2015</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13">
+        <v>36</v>
+      </c>
+      <c r="E13">
+        <v>11341</v>
+      </c>
+      <c r="H13" s="1">
+        <v>42252</v>
+      </c>
+      <c r="I13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13">
+        <v>96</v>
+      </c>
+      <c r="L13">
+        <v>88</v>
+      </c>
+      <c r="M13">
+        <v>66</v>
+      </c>
+      <c r="N13">
+        <v>22</v>
+      </c>
+      <c r="O13">
+        <v>25</v>
+      </c>
+      <c r="P13" t="s">
+        <v>80</v>
+      </c>
+      <c r="R13">
+        <v>66</v>
+      </c>
+      <c r="S13">
+        <v>22</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="V13">
+        <v>36</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2014</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14">
+        <v>36</v>
+      </c>
+      <c r="E14">
+        <v>11341</v>
+      </c>
+      <c r="H14" s="1">
+        <v>41884</v>
+      </c>
+      <c r="I14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14">
+        <v>96</v>
+      </c>
+      <c r="L14">
+        <v>92</v>
+      </c>
+      <c r="M14">
+        <v>39</v>
+      </c>
+      <c r="N14">
+        <v>53</v>
+      </c>
+      <c r="O14">
+        <v>58</v>
+      </c>
+      <c r="P14" t="s">
+        <v>80</v>
+      </c>
+      <c r="R14">
+        <v>39</v>
+      </c>
+      <c r="S14">
+        <v>53</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="2"/>
+        <v>0.57608695652173914</v>
+      </c>
+      <c r="V14">
+        <v>36</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="0"/>
+        <v>0.57608695652173914</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15">
+        <v>36</v>
+      </c>
+      <c r="E15">
+        <v>11341</v>
+      </c>
+      <c r="H15" s="1">
+        <v>41519</v>
+      </c>
+      <c r="I15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15">
+        <v>96</v>
+      </c>
+      <c r="L15">
+        <v>94</v>
+      </c>
+      <c r="M15">
+        <v>72</v>
+      </c>
+      <c r="N15">
+        <v>22</v>
+      </c>
+      <c r="O15">
+        <v>23</v>
+      </c>
+      <c r="P15" t="s">
+        <v>80</v>
+      </c>
+      <c r="R15">
+        <v>72</v>
+      </c>
+      <c r="S15">
+        <v>22</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="2"/>
+        <v>0.23404255319148937</v>
+      </c>
+      <c r="V15">
+        <v>36</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="0"/>
+        <v>0.23404255319148937</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2012</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16">
+        <v>37</v>
+      </c>
+      <c r="E16">
+        <v>11336</v>
+      </c>
+      <c r="H16" s="1">
+        <v>41167</v>
+      </c>
+      <c r="I16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16">
+        <v>96</v>
+      </c>
+      <c r="L16">
+        <v>94</v>
+      </c>
+      <c r="M16">
+        <v>77</v>
+      </c>
+      <c r="N16">
+        <v>17</v>
+      </c>
+      <c r="O16">
+        <v>18</v>
+      </c>
+      <c r="P16" t="s">
+        <v>80</v>
+      </c>
+      <c r="R16">
+        <v>77</v>
+      </c>
+      <c r="S16">
+        <v>17</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="2"/>
+        <v>0.18085106382978725</v>
+      </c>
+      <c r="V16">
+        <v>37</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="0"/>
+        <v>0.18085106382978725</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2011</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17">
+        <v>38</v>
+      </c>
+      <c r="E17">
+        <v>11336</v>
+      </c>
+      <c r="H17" s="1">
+        <v>40800</v>
+      </c>
+      <c r="I17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17">
+        <v>96</v>
+      </c>
+      <c r="L17">
+        <v>94</v>
+      </c>
+      <c r="M17">
+        <v>86</v>
+      </c>
+      <c r="N17">
+        <v>8</v>
+      </c>
+      <c r="O17">
+        <v>9</v>
+      </c>
+      <c r="P17" t="s">
+        <v>80</v>
+      </c>
+      <c r="R17">
+        <v>86</v>
+      </c>
+      <c r="S17">
+        <v>8</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="2"/>
+        <v>8.5106382978723402E-2</v>
+      </c>
+      <c r="V17">
+        <v>38</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="0"/>
+        <v>8.5106382978723402E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2024</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20">
+        <v>32</v>
+      </c>
+      <c r="E20">
+        <v>90</v>
+      </c>
+      <c r="F20">
+        <v>137</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G35" si="3">E20/F20</f>
+        <v>0.65693430656934304</v>
+      </c>
+      <c r="I20" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20">
+        <v>32</v>
+      </c>
+      <c r="K20">
+        <v>0.65693430656934304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2024</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21">
+        <v>33</v>
+      </c>
+      <c r="E21">
+        <v>81</v>
+      </c>
+      <c r="F21">
+        <v>135</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="I21" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21">
+        <v>33</v>
+      </c>
+      <c r="K21">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2021</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22">
+        <v>36</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>31</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22">
+        <v>33</v>
+      </c>
+      <c r="K22">
+        <v>0.77272727272727271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2021</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23">
+        <v>36</v>
+      </c>
+      <c r="E23">
+        <v>29</v>
+      </c>
+      <c r="F23">
+        <v>32</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>0.90625</v>
+      </c>
+      <c r="I23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23">
+        <v>34</v>
+      </c>
+      <c r="K23">
+        <v>0.88659793814432986</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2020</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>33</v>
+      </c>
+      <c r="E24">
+        <v>51</v>
+      </c>
+      <c r="F24">
+        <v>66</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="I24" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24">
+        <v>30</v>
+      </c>
+      <c r="K24">
+        <v>0.95121951219512191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2019</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25">
+        <v>34</v>
+      </c>
+      <c r="E25">
+        <v>86</v>
+      </c>
+      <c r="F25">
+        <v>97</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>0.88659793814432986</v>
+      </c>
+      <c r="I25" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25">
+        <v>34</v>
+      </c>
+      <c r="K25">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2017</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>78</v>
+      </c>
+      <c r="F26">
+        <v>82</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>0.95121951219512191</v>
+      </c>
+      <c r="I26" t="s">
+        <v>54</v>
+      </c>
+      <c r="J26">
+        <v>36</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2017</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27">
+        <v>37</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <v>14</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="I27" t="s">
+        <v>54</v>
+      </c>
+      <c r="J27">
+        <v>36</v>
+      </c>
+      <c r="K27">
+        <v>0.90625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2017</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28">
+        <v>38</v>
+      </c>
+      <c r="E28">
+        <v>32</v>
+      </c>
+      <c r="F28">
+        <v>69</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>0.46376811594202899</v>
+      </c>
+      <c r="I28" t="s">
+        <v>54</v>
+      </c>
+      <c r="J28">
+        <v>37</v>
+      </c>
+      <c r="K28">
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2016</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29">
+        <v>34</v>
+      </c>
+      <c r="E29">
+        <v>46</v>
+      </c>
+      <c r="F29">
+        <v>50</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>0.92</v>
+      </c>
+      <c r="I29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J29">
+        <v>38</v>
+      </c>
+      <c r="K29">
+        <v>0.46376811594202899</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2016</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30">
+        <v>36</v>
+      </c>
+      <c r="E30">
+        <v>46</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>0.92</v>
+      </c>
+      <c r="I30" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30">
+        <v>36</v>
+      </c>
+      <c r="K30">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2015</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31">
+        <v>36</v>
+      </c>
+      <c r="E31">
+        <v>22</v>
+      </c>
+      <c r="F31">
+        <v>88</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="I31" t="s">
+        <v>54</v>
+      </c>
+      <c r="J31">
+        <v>36</v>
+      </c>
+      <c r="K31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2014</v>
+      </c>
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32">
+        <v>36</v>
+      </c>
+      <c r="E32">
+        <v>53</v>
+      </c>
+      <c r="F32">
+        <v>92</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>0.57608695652173914</v>
+      </c>
+      <c r="I32" t="s">
+        <v>54</v>
+      </c>
+      <c r="J32">
+        <v>36</v>
+      </c>
+      <c r="K32">
+        <v>0.57608695652173914</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2013</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33">
+        <v>36</v>
+      </c>
+      <c r="E33">
+        <v>22</v>
+      </c>
+      <c r="F33">
+        <v>94</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>0.23404255319148937</v>
+      </c>
+      <c r="I33" t="s">
+        <v>54</v>
+      </c>
+      <c r="J33">
+        <v>36</v>
+      </c>
+      <c r="K33">
+        <v>0.23404255319148937</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2012</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34">
+        <v>37</v>
+      </c>
+      <c r="E34">
+        <v>17</v>
+      </c>
+      <c r="F34">
+        <v>94</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>0.18085106382978725</v>
+      </c>
+      <c r="I34" t="s">
+        <v>54</v>
+      </c>
+      <c r="J34">
+        <v>37</v>
+      </c>
+      <c r="K34">
+        <v>0.18085106382978725</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2011</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35">
+        <v>38</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <v>94</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>8.5106382978723402E-2</v>
+      </c>
+      <c r="I35" t="s">
+        <v>54</v>
+      </c>
+      <c r="J35">
+        <v>38</v>
+      </c>
+      <c r="K35">
+        <v>8.5106382978723402E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I20:K35">
+    <sortCondition ref="I19:I35"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F84DE98-9CB9-44EA-83F5-0A38140FF06A}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AH108"/>
@@ -21667,11 +24371,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF69900-6BF5-40CF-908D-6F67556CB845}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -22232,7 +24936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B4DDE9-1032-4410-8A30-58DADF58182E}">
   <dimension ref="A2:S16"/>
   <sheetViews>

</xml_diff>

<commit_message>
changes to excel stuff
</commit_message>
<xml_diff>
--- a/data/raw/ADFG_strayrates.xlsx
+++ b/data/raw/ADFG_strayrates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thema\OneDrive\Documents\dissertation\SITK\Github\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0087409-211D-40B4-A224-2D709A2CF88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F77A85-727D-4B3B-B5F6-E39AFC0BE2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-52920" yWindow="-375" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{28766EB7-7A80-4306-B235-966A57E0829F}"/>
   </bookViews>
@@ -2452,7 +2452,67 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Timing of SJH stray</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> rate analysis by category</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -16928,7 +16988,7 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W33" sqref="W33"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>